<commit_message>
links, jump function and full screen mode
</commit_message>
<xml_diff>
--- a/ablaufplan.xlsx
+++ b/ablaufplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsf\Programmieren\Script4Fun\S4F_Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69BF94E-1607-4B84-9215-575FBBEB971A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6B45EC-403A-4CE4-95D1-1DAACE21D414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BAD20FD-7C3F-4F70-BFFC-FB793AF94706}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Schritte</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Projekt von Nils Fischer</t>
+  </si>
+  <si>
+    <t>18.05.</t>
   </si>
 </sst>
 </file>
@@ -445,13 +448,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -503,6 +499,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20 % - Akzent4" xfId="2" builtinId="42"/>
@@ -845,7 +848,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,36 +867,36 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="55"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="55"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="55"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="55"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="53"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -910,209 +913,209 @@
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="20"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="20"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="20"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="20"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="20"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="20"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="20"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="20"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="20"/>
-    </row>
-    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="17"/>
+    </row>
+    <row r="14" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="31"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="22"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="28"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="20"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:14" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="37" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="15">
-        <v>18.25</v>
+      <c r="F16" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>14</v>
@@ -1172,7 +1175,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1189,7 +1192,7 @@
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="50">
         <v>45037</v>
       </c>
       <c r="C4" s="10">
@@ -1212,7 +1215,7 @@
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="50">
         <v>45037</v>
       </c>
       <c r="C5" s="10">
@@ -1227,7 +1230,7 @@
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="50">
         <v>45046</v>
       </c>
       <c r="C6" s="10"/>
@@ -1240,7 +1243,7 @@
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="50">
         <v>45053</v>
       </c>
       <c r="C7" s="10"/>
@@ -1253,7 +1256,7 @@
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="50">
         <v>45078</v>
       </c>
       <c r="C8" s="10"/>
@@ -1266,7 +1269,7 @@
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="50">
         <v>45085</v>
       </c>
       <c r="C9" s="10"/>
@@ -1279,7 +1282,7 @@
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="50">
         <v>45078</v>
       </c>
       <c r="C10" s="10"/>
@@ -1292,7 +1295,7 @@
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B11" s="50">
         <v>45092</v>
       </c>
       <c r="C11" s="10"/>
@@ -1305,7 +1308,7 @@
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="50">
         <v>45106</v>
       </c>
       <c r="C12" s="10"/>
@@ -1315,10 +1318,10 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="50">
         <v>45106</v>
       </c>
       <c r="C13" s="10"/>
@@ -1331,7 +1334,7 @@
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="50">
         <v>45106</v>
       </c>
       <c r="C14" s="10"/>
@@ -1341,7 +1344,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="52"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D14">

</xml_diff>